<commit_message>
Added test for opaque (#225)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
   <si>
     <t xml:space="preserve">Contexts</t>
   </si>
@@ -366,8 +366,8 @@
   </sheetPr>
   <dimension ref="A1:Y15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O17" activeCellId="0" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -549,12 +549,16 @@
       <c r="Q3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="R3" s="5"/>
+      <c r="R3" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="S3" s="5"/>
       <c r="T3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="U3" s="5"/>
+      <c r="U3" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="V3" s="6"/>
       <c r="W3" s="6"/>
       <c r="X3" s="5" t="s">
@@ -934,7 +938,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added bool test case (#225)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="38">
   <si>
     <t xml:space="preserve">Contexts</t>
   </si>
@@ -367,7 +367,7 @@
   <dimension ref="A1:Y15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O17" activeCellId="0" sqref="O17"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -515,7 +515,9 @@
       <c r="C3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="5"/>
+      <c r="D3" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="E3" s="5" t="s">
         <v>27</v>
       </c>
@@ -938,7 +940,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added tests for array and pointer (#225)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
   <si>
     <t xml:space="preserve">Contexts</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t xml:space="preserve">Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x</t>
   </si>
   <si>
     <t xml:space="preserve">As function parameters</t>
@@ -176,7 +179,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -193,6 +196,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
@@ -250,7 +259,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -275,7 +284,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -367,7 +384,7 @@
   <dimension ref="A1:Y15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -527,9 +544,15 @@
       <c r="G3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
+      <c r="H3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="K3" s="5" t="s">
         <v>27</v>
       </c>
@@ -554,15 +577,17 @@
       <c r="R3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="S3" s="5"/>
+      <c r="S3" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="T3" s="5" t="s">
         <v>27</v>
       </c>
       <c r="U3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
       <c r="X3" s="5" t="s">
         <v>27</v>
       </c>
@@ -572,7 +597,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -601,7 +626,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -630,7 +655,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -659,7 +684,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -688,7 +713,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -717,7 +742,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -746,7 +771,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -754,7 +779,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
-      <c r="H10" s="7"/>
+      <c r="H10" s="9"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
@@ -775,7 +800,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -804,7 +829,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -833,7 +858,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -861,7 +886,7 @@
       <c r="Y13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8"/>
+      <c r="A14" s="10"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -888,7 +913,7 @@
       <c r="Y14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8"/>
+      <c r="A15" s="10"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -940,7 +965,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added more tests (#225)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="38">
   <si>
     <t xml:space="preserve">Contexts</t>
   </si>
@@ -105,9 +105,6 @@
   </si>
   <si>
     <t xml:space="preserve">Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x</t>
   </si>
   <si>
     <t xml:space="preserve">As function parameters</t>
@@ -147,7 +144,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -178,8 +175,14 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -196,12 +199,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor rgb="FFC0C0C0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
@@ -288,11 +285,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -384,7 +381,7 @@
   <dimension ref="A1:Y15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
+      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -544,14 +541,14 @@
       <c r="G3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>28</v>
+      <c r="H3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>27</v>
@@ -578,7 +575,7 @@
         <v>27</v>
       </c>
       <c r="S3" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="T3" s="5" t="s">
         <v>27</v>
@@ -597,7 +594,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -607,7 +604,9 @@
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
+      <c r="J4" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
@@ -626,7 +625,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -655,7 +654,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -684,7 +683,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -713,7 +712,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -742,7 +741,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -771,7 +770,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -800,7 +799,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -829,7 +828,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -858,7 +857,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -965,7 +964,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added support for getters/setters (#234)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -10,6 +10,10 @@
   <sheets>
     <sheet name="Type handling" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Console" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Crypto" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Error handling" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Function calling" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Memory allocation" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,12 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="40">
-  <si>
-    <t xml:space="preserve">Contexts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Types</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="47">
+  <si>
+    <t xml:space="preserve">Context</t>
   </si>
   <si>
     <t xml:space="preserve">Type</t>
@@ -141,6 +142,30 @@
   </si>
   <si>
     <t xml:space="preserve">Vector of</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scenario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Print with newline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Print without newline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generate md5 hash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generate sha1 hash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASM error trace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attach getters/setters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create internal slice</t>
   </si>
 </sst>
 </file>
@@ -188,7 +213,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -203,8 +228,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF81D41A"/>
+        <bgColor rgb="FF92D050"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor rgb="FFC0C0C0"/>
+        <bgColor rgb="FF81D41A"/>
       </patternFill>
     </fill>
     <fill>
@@ -274,7 +305,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -287,7 +318,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -296,27 +327,31 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -344,7 +379,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF92D050"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -372,7 +407,7 @@
       <rgbColor rgb="FFFFD8CE"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF92D050"/>
+      <rgbColor rgb="FF81D41A"/>
       <rgbColor rgb="FFFFC000"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
@@ -399,7 +434,7 @@
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T4" activeCellId="0" sqref="T4"/>
+      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -465,868 +500,868 @@
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S3" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T3" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="V3" s="7"/>
       <c r="W3" s="7"/>
       <c r="X3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Y3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J4" s="5"/>
       <c r="K4" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S4" s="5"/>
       <c r="T4" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="U4" s="5"/>
       <c r="V4" s="7"/>
       <c r="W4" s="7"/>
       <c r="X4" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Y4" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S5" s="5"/>
       <c r="T5" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="U5" s="5"/>
       <c r="V5" s="7"/>
       <c r="W5" s="7"/>
       <c r="X5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Y5" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P6" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q6" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R6" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S6" s="5"/>
       <c r="T6" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="U6" s="5"/>
       <c r="V6" s="7"/>
       <c r="W6" s="7"/>
       <c r="X6" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Y6" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J7" s="5"/>
       <c r="K7" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M7" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P7" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q7" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R7" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S7" s="5"/>
       <c r="T7" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="U7" s="5"/>
       <c r="V7" s="7"/>
       <c r="W7" s="7"/>
       <c r="X7" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Y7" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J8" s="5"/>
       <c r="K8" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R8" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S8" s="5"/>
       <c r="T8" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="U8" s="5"/>
       <c r="V8" s="7"/>
       <c r="W8" s="7"/>
       <c r="X8" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Y8" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H9" s="5"/>
       <c r="I9" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J9" s="5"/>
       <c r="K9" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M9" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O9" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P9" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q9" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R9" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S9" s="5"/>
       <c r="T9" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="U9" s="5"/>
       <c r="V9" s="7"/>
       <c r="W9" s="7"/>
       <c r="X9" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Y9" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J10" s="5"/>
       <c r="K10" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M10" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q10" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R10" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S10" s="5"/>
       <c r="T10" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="U10" s="5"/>
       <c r="V10" s="7"/>
       <c r="W10" s="7"/>
       <c r="X10" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Y10" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H11" s="10"/>
       <c r="I11" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J11" s="5"/>
       <c r="K11" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M11" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O11" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P11" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q11" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R11" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S11" s="5"/>
       <c r="T11" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="U11" s="5"/>
       <c r="V11" s="7"/>
       <c r="W11" s="7"/>
       <c r="X11" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Y11" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J12" s="5"/>
       <c r="K12" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M12" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O12" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P12" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q12" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R12" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S12" s="5"/>
       <c r="T12" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="U12" s="5"/>
       <c r="V12" s="7"/>
       <c r="W12" s="7"/>
       <c r="X12" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Y12" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J13" s="5"/>
       <c r="K13" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N13" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O13" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P13" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q13" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R13" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S13" s="5"/>
       <c r="T13" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="U13" s="5"/>
       <c r="V13" s="7"/>
       <c r="W13" s="7"/>
       <c r="X13" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Y13" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J14" s="5"/>
       <c r="K14" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N14" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O14" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P14" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q14" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R14" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S14" s="5"/>
       <c r="T14" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="U14" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="V14" s="7"/>
       <c r="W14" s="7"/>
       <c r="X14" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Y14" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1351,14 +1386,264 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="11"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="11"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="11"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="11"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="11"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="11"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="11"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="11"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="11"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="11"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Incorporated old tests into new scheme (#225)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="59">
   <si>
     <t xml:space="preserve">Context</t>
   </si>
@@ -162,10 +162,46 @@
     <t xml:space="preserve">WASM error trace</t>
   </si>
   <si>
+    <t xml:space="preserve">Throw error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Return slice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Return slice of slices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Print slice of slices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accept typed array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Return bool vector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Handle misaligned pointer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Handled misaligned aliased pointer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allocate slice of structs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clear pointers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clear pointer array</t>
+  </si>
+  <si>
     <t xml:space="preserve">Attach getters/setters</t>
   </si>
   <si>
     <t xml:space="preserve">Create internal slice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allocate memory for string</t>
   </si>
 </sst>
 </file>
@@ -434,7 +470,7 @@
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
+      <selection pane="topLeft" activeCell="J14" activeCellId="0" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1500,10 +1536,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1528,10 +1564,6 @@
       <c r="B3" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1553,15 +1585,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.06"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1583,8 +1615,92 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
+      <c r="A4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1609,7 +1725,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1629,15 +1745,19 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
+      <c r="A4" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Implemented const objects (#26)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -341,7 +341,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -371,6 +371,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -470,7 +474,7 @@
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J14" activeCellId="0" sqref="J14"/>
+      <selection pane="topLeft" activeCell="M21" activeCellId="0" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -798,7 +802,7 @@
         <v>26</v>
       </c>
       <c r="S5" s="5"/>
-      <c r="T5" s="8" t="s">
+      <c r="T5" s="9" t="s">
         <v>27</v>
       </c>
       <c r="U5" s="5"/>
@@ -815,7 +819,7 @@
       <c r="A6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="9" t="s">
         <v>26</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -840,10 +844,10 @@
       <c r="J6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K6" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="L6" s="9" t="s">
+      <c r="K6" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" s="10" t="s">
         <v>26</v>
       </c>
       <c r="M6" s="5" t="s">
@@ -865,7 +869,7 @@
         <v>26</v>
       </c>
       <c r="S6" s="5"/>
-      <c r="T6" s="8" t="s">
+      <c r="T6" s="9" t="s">
         <v>27</v>
       </c>
       <c r="U6" s="5"/>
@@ -874,7 +878,7 @@
       <c r="X6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="Y6" s="8" t="s">
+      <c r="Y6" s="9" t="s">
         <v>26</v>
       </c>
     </row>
@@ -905,13 +909,13 @@
         <v>26</v>
       </c>
       <c r="J7" s="5"/>
-      <c r="K7" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="L7" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="M7" s="8" t="s">
+      <c r="K7" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" s="9" t="s">
         <v>26</v>
       </c>
       <c r="N7" s="5" t="s">
@@ -939,7 +943,7 @@
       <c r="X7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="Y7" s="8" t="s">
+      <c r="Y7" s="9" t="s">
         <v>26</v>
       </c>
     </row>
@@ -991,17 +995,17 @@
       <c r="Q8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="R8" s="8" t="s">
+      <c r="R8" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S8" s="5"/>
-      <c r="T8" s="8" t="s">
+      <c r="T8" s="9" t="s">
         <v>27</v>
       </c>
       <c r="U8" s="5"/>
       <c r="V8" s="7"/>
       <c r="W8" s="7"/>
-      <c r="X8" s="8" t="s">
+      <c r="X8" s="9" t="s">
         <v>26</v>
       </c>
       <c r="Y8" s="5" t="s">
@@ -1041,7 +1045,7 @@
       <c r="L9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="M9" s="8" t="s">
+      <c r="M9" s="9" t="s">
         <v>26</v>
       </c>
       <c r="N9" s="5" t="s">
@@ -1053,14 +1057,14 @@
       <c r="P9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="Q9" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="R9" s="8" t="s">
+      <c r="Q9" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="R9" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S9" s="5"/>
-      <c r="T9" s="8" t="s">
+      <c r="T9" s="9" t="s">
         <v>27</v>
       </c>
       <c r="U9" s="5"/>
@@ -1077,7 +1081,7 @@
       <c r="A10" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="9" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -1100,13 +1104,13 @@
         <v>26</v>
       </c>
       <c r="J10" s="5"/>
-      <c r="K10" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="M10" s="8" t="s">
+      <c r="K10" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="M10" s="9" t="s">
         <v>27</v>
       </c>
       <c r="N10" s="5" t="s">
@@ -1134,7 +1138,7 @@
       <c r="X10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="Y10" s="8" t="s">
+      <c r="Y10" s="9" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1142,7 +1146,7 @@
       <c r="A11" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="9" t="s">
         <v>26</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -1160,18 +1164,18 @@
       <c r="G11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="10"/>
+      <c r="H11" s="11"/>
       <c r="I11" s="5" t="s">
         <v>26</v>
       </c>
       <c r="J11" s="5"/>
-      <c r="K11" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="L11" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="M11" s="8" t="s">
+      <c r="K11" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="M11" s="9" t="s">
         <v>27</v>
       </c>
       <c r="N11" s="5" t="s">
@@ -1199,7 +1203,7 @@
       <c r="X11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="Y11" s="8" t="s">
+      <c r="Y11" s="9" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1207,7 +1211,7 @@
       <c r="A12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="9" t="s">
         <v>26</v>
       </c>
       <c r="C12" s="5" t="s">
@@ -1230,10 +1234,10 @@
         <v>26</v>
       </c>
       <c r="J12" s="5"/>
-      <c r="K12" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="L12" s="8" t="s">
+      <c r="K12" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L12" s="9" t="s">
         <v>26</v>
       </c>
       <c r="M12" s="5" t="s">
@@ -1248,7 +1252,7 @@
       <c r="P12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="Q12" s="8" t="s">
+      <c r="Q12" s="9" t="s">
         <v>26</v>
       </c>
       <c r="R12" s="5" t="s">
@@ -1264,7 +1268,7 @@
       <c r="X12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="Y12" s="8" t="s">
+      <c r="Y12" s="9" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1272,7 +1276,7 @@
       <c r="A13" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="9" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="5" t="s">
@@ -1295,10 +1299,10 @@
         <v>26</v>
       </c>
       <c r="J13" s="5"/>
-      <c r="K13" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="L13" s="8" t="s">
+      <c r="K13" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L13" s="9" t="s">
         <v>26</v>
       </c>
       <c r="M13" s="5" t="s">
@@ -1310,7 +1314,7 @@
       <c r="O13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="P13" s="8" t="s">
+      <c r="P13" s="9" t="s">
         <v>26</v>
       </c>
       <c r="Q13" s="5" t="s">
@@ -1329,7 +1333,7 @@
       <c r="X13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="Y13" s="8" t="s">
+      <c r="Y13" s="9" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1437,11 +1441,11 @@
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="12"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="11"/>
+      <c r="B2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -1494,11 +1498,11 @@
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="12"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="11"/>
+      <c r="B2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -1551,11 +1555,11 @@
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="12"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="11"/>
+      <c r="B2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -1600,11 +1604,11 @@
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="12"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="11"/>
+      <c r="B2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -1737,11 +1741,11 @@
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="12"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="11"/>
+      <c r="B2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">

</xml_diff>

<commit_message>
Added some tests for union (#225)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="59">
   <si>
     <t xml:space="preserve">Context</t>
   </si>
@@ -470,7 +470,7 @@
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
+      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -734,7 +734,9 @@
       <c r="R4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="S4" s="5"/>
+      <c r="S4" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="T4" s="5" t="s">
         <v>27</v>
       </c>
@@ -801,7 +803,9 @@
       <c r="R5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="S5" s="5"/>
+      <c r="S5" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="T5" s="8" t="s">
         <v>27</v>
       </c>
@@ -868,7 +872,9 @@
       <c r="R6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="S6" s="5"/>
+      <c r="S6" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="T6" s="8" t="s">
         <v>27</v>
       </c>
@@ -1270,7 +1276,9 @@
       <c r="R12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="S12" s="5"/>
+      <c r="S12" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="T12" s="5" t="s">
         <v>27</v>
       </c>
@@ -1337,7 +1345,9 @@
       <c r="R13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="S13" s="5"/>
+      <c r="S13" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="T13" s="5" t="s">
         <v>27</v>
       </c>
@@ -1378,7 +1388,7 @@
         <v>27</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K14" s="5" t="s">
         <v>27</v>
@@ -1404,7 +1414,9 @@
       <c r="R14" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="S14" s="5"/>
+      <c r="S14" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="T14" s="5" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Implemented fixed object (#233)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="60">
   <si>
     <t xml:space="preserve">Context</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t xml:space="preserve">Allocate memory for string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create fixed object</t>
   </si>
 </sst>
 </file>
@@ -341,7 +344,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -379,10 +382,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -997,7 +996,7 @@
       <c r="G8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="5" t="s">
         <v>27</v>
       </c>
       <c r="I8" s="5" t="s">
@@ -1210,7 +1209,7 @@
       <c r="G11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="10" t="s">
         <v>26</v>
       </c>
       <c r="I11" s="5" t="s">
@@ -1515,11 +1514,11 @@
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="12"/>
+      <c r="B2" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -1572,11 +1571,11 @@
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="12"/>
+      <c r="B2" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -1629,11 +1628,11 @@
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="12"/>
+      <c r="B2" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -1678,11 +1677,11 @@
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="12"/>
+      <c r="B2" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -1800,10 +1799,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1815,11 +1814,11 @@
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="12"/>
+      <c r="B2" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -1834,6 +1833,14 @@
         <v>58</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ADjusted code to deal with self-referencing struct (#220)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Type handling" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="62">
   <si>
     <t xml:space="preserve">Context</t>
   </si>
@@ -196,6 +196,12 @@
   </si>
   <si>
     <t xml:space="preserve">Attach getters/setters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Return self-referencing struct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Return same struct</t>
   </si>
   <si>
     <t xml:space="preserve">Create internal slice</t>
@@ -472,7 +478,7 @@
   </sheetPr>
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -1662,10 +1668,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1776,6 +1782,22 @@
         <v>56</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1822,7 +1844,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>26</v>
@@ -1830,7 +1852,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>26</v>
@@ -1838,7 +1860,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Fixed union handling (#243)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Type handling" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="62">
   <si>
     <t xml:space="preserve">Context</t>
   </si>
@@ -350,7 +350,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -388,6 +388,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -478,8 +482,8 @@
   </sheetPr>
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -891,7 +895,7 @@
       <c r="R6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="S6" s="8" t="s">
+      <c r="S6" s="10" t="s">
         <v>26</v>
       </c>
       <c r="T6" s="8" t="s">
@@ -964,7 +968,9 @@
       <c r="R7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="S7" s="5"/>
+      <c r="S7" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="T7" s="5" t="s">
         <v>27</v>
       </c>
@@ -1035,7 +1041,9 @@
       <c r="R8" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="S8" s="5"/>
+      <c r="S8" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="T8" s="8" t="s">
         <v>27</v>
       </c>
@@ -1106,7 +1114,9 @@
       <c r="R9" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="S9" s="5"/>
+      <c r="S9" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="T9" s="8" t="s">
         <v>27</v>
       </c>
@@ -1177,7 +1187,9 @@
       <c r="R10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="S10" s="5"/>
+      <c r="S10" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="T10" s="5" t="s">
         <v>27</v>
       </c>
@@ -1215,7 +1227,7 @@
       <c r="G11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="11" t="s">
         <v>26</v>
       </c>
       <c r="I11" s="5" t="s">
@@ -1248,7 +1260,9 @@
       <c r="R11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="S11" s="5"/>
+      <c r="S11" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="T11" s="5" t="s">
         <v>27</v>
       </c>
@@ -1319,7 +1333,7 @@
       <c r="R12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="S12" s="8" t="s">
+      <c r="S12" s="10" t="s">
         <v>26</v>
       </c>
       <c r="T12" s="5" t="s">
@@ -1392,7 +1406,7 @@
       <c r="R13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="S13" s="8" t="s">
+      <c r="S13" s="10" t="s">
         <v>26</v>
       </c>
       <c r="T13" s="5" t="s">
@@ -1520,11 +1534,11 @@
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="12"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="11"/>
+      <c r="B2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -1577,11 +1591,11 @@
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="12"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="11"/>
+      <c r="B2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -1634,11 +1648,11 @@
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="12"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="11"/>
+      <c r="B2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -1670,7 +1684,7 @@
   </sheetPr>
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
     </sheetView>
   </sheetViews>
@@ -1683,11 +1697,11 @@
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="12"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="11"/>
+      <c r="B2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -1836,11 +1850,11 @@
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="12"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="11"/>
+      <c r="B2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">

</xml_diff>

<commit_message>
Allowing pointer to self in method calls (#242)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="63">
   <si>
     <t xml:space="preserve">Context</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t xml:space="preserve">Return same struct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allow call as methods</t>
   </si>
   <si>
     <t xml:space="preserve">Create internal slice</t>
@@ -350,7 +353,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -388,10 +391,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -895,7 +894,7 @@
       <c r="R6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="S6" s="10" t="s">
+      <c r="S6" s="5" t="s">
         <v>26</v>
       </c>
       <c r="T6" s="8" t="s">
@@ -1227,7 +1226,7 @@
       <c r="G11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="10" t="s">
         <v>26</v>
       </c>
       <c r="I11" s="5" t="s">
@@ -1333,7 +1332,7 @@
       <c r="R12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="S12" s="10" t="s">
+      <c r="S12" s="5" t="s">
         <v>26</v>
       </c>
       <c r="T12" s="5" t="s">
@@ -1406,7 +1405,7 @@
       <c r="R13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="S13" s="10" t="s">
+      <c r="S13" s="5" t="s">
         <v>26</v>
       </c>
       <c r="T13" s="5" t="s">
@@ -1534,11 +1533,11 @@
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="12"/>
+      <c r="B2" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -1591,11 +1590,11 @@
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="12"/>
+      <c r="B2" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -1648,11 +1647,11 @@
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="12"/>
+      <c r="B2" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -1682,10 +1681,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1697,11 +1696,11 @@
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="12"/>
+      <c r="B2" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -1812,6 +1811,14 @@
         <v>58</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1850,15 +1857,15 @@
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="12"/>
+      <c r="B2" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>26</v>
@@ -1866,7 +1873,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>26</v>
@@ -1874,7 +1881,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Began fixing comptime numbers (#237)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -353,7 +353,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -395,6 +395,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -482,7 +486,7 @@
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="L10" activeCellId="0" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1308,10 +1312,10 @@
       <c r="J12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K12" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="L12" s="8" t="s">
+      <c r="K12" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="L12" s="11" t="s">
         <v>26</v>
       </c>
       <c r="M12" s="5" t="s">
@@ -1533,11 +1537,11 @@
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="12"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="11"/>
+      <c r="B2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -1590,11 +1594,11 @@
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="12"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="11"/>
+      <c r="B2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -1647,11 +1651,11 @@
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="12"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="11"/>
+      <c r="B2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -1696,11 +1700,11 @@
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="12"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="11"/>
+      <c r="B2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -1857,11 +1861,11 @@
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="12"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="11"/>
+      <c r="B2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">

</xml_diff>

<commit_message>
Allowing comptime numbers in tagged union (#237)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -261,7 +261,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -295,13 +295,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFD8CE"/>
-        <bgColor rgb="FFFFD7D7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFD7D7"/>
-        <bgColor rgb="FFFFD8CE"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -353,7 +347,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -387,10 +381,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -435,7 +425,7 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFD7D7"/>
+      <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
@@ -486,7 +476,7 @@
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L10" activeCellId="0" sqref="L10"/>
+      <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -874,10 +864,10 @@
       <c r="J6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K6" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="L6" s="9" t="s">
+      <c r="K6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" s="5" t="s">
         <v>26</v>
       </c>
       <c r="M6" s="5" t="s">
@@ -947,10 +937,10 @@
       <c r="J7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K7" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="L7" s="8" t="s">
+      <c r="K7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L7" s="5" t="s">
         <v>26</v>
       </c>
       <c r="M7" s="8" t="s">
@@ -1093,10 +1083,10 @@
       <c r="J9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K9" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L9" s="5" t="s">
+      <c r="K9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9" s="8" t="s">
         <v>26</v>
       </c>
       <c r="M9" s="8" t="s">
@@ -1230,7 +1220,7 @@
       <c r="G11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="9" t="s">
         <v>26</v>
       </c>
       <c r="I11" s="5" t="s">
@@ -1239,10 +1229,10 @@
       <c r="J11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K11" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="L11" s="8" t="s">
+      <c r="K11" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="L11" s="10" t="s">
         <v>26</v>
       </c>
       <c r="M11" s="8" t="s">
@@ -1312,10 +1302,10 @@
       <c r="J12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K12" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="L12" s="11" t="s">
+      <c r="K12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L12" s="5" t="s">
         <v>26</v>
       </c>
       <c r="M12" s="5" t="s">
@@ -1385,10 +1375,10 @@
       <c r="J13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K13" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="L13" s="8" t="s">
+      <c r="K13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L13" s="5" t="s">
         <v>26</v>
       </c>
       <c r="M13" s="5" t="s">
@@ -1537,11 +1527,11 @@
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="12"/>
+      <c r="B2" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -1594,11 +1584,11 @@
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="12"/>
+      <c r="B2" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -1651,11 +1641,11 @@
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="12"/>
+      <c r="B2" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -1700,11 +1690,11 @@
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="12"/>
+      <c r="B2" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -1861,11 +1851,11 @@
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="12"/>
+      <c r="B2" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">

</xml_diff>

<commit_message>
Fixed regression with comptime numbers (#237)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -384,11 +384,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -476,7 +476,7 @@
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
+      <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1083,10 +1083,10 @@
       <c r="J9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K9" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="L9" s="8" t="s">
+      <c r="K9" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9" s="9" t="s">
         <v>26</v>
       </c>
       <c r="M9" s="8" t="s">
@@ -1220,7 +1220,7 @@
       <c r="G11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H11" s="10" t="s">
         <v>26</v>
       </c>
       <c r="I11" s="5" t="s">
@@ -1229,10 +1229,10 @@
       <c r="J11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K11" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="L11" s="10" t="s">
+      <c r="K11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L11" s="5" t="s">
         <v>26</v>
       </c>
       <c r="M11" s="8" t="s">

</xml_diff>

<commit_message>
Reworking how comptime values are handled (#238)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -476,7 +476,11 @@
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="Q3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="Q1" activeCellId="0" sqref="Q1"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="Y13" activeCellId="0" sqref="Y13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -683,7 +687,7 @@
       <c r="X3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="Y3" s="5" t="s">
+      <c r="Y3" s="8" t="s">
         <v>26</v>
       </c>
     </row>
@@ -975,7 +979,7 @@
       <c r="X7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="Y7" s="8" t="s">
+      <c r="Y7" s="9" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1083,10 +1087,10 @@
       <c r="J9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K9" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="L9" s="9" t="s">
+      <c r="K9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9" s="5" t="s">
         <v>26</v>
       </c>
       <c r="M9" s="8" t="s">
@@ -1267,7 +1271,7 @@
       <c r="X11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="Y11" s="8" t="s">
+      <c r="Y11" s="9" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1340,7 +1344,7 @@
       <c r="X12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="Y12" s="8" t="s">
+      <c r="Y12" s="9" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Enabled array of types (#238)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -476,11 +476,11 @@
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="Q3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="Q1" activeCellId="0" sqref="Q1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Y13" activeCellId="0" sqref="Y13"/>
+      <selection pane="bottomRight" activeCell="F8" activeCellId="0" sqref="F8:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -696,7 +696,7 @@
         <v>28</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>26</v>
@@ -769,7 +769,7 @@
         <v>29</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>26</v>
@@ -841,7 +841,7 @@
       <c r="A6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -906,7 +906,7 @@
       <c r="X6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="Y6" s="8" t="s">
+      <c r="Y6" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -915,7 +915,7 @@
         <v>31</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>26</v>
@@ -979,7 +979,7 @@
       <c r="X7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="Y7" s="9" t="s">
+      <c r="Y7" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -999,10 +999,10 @@
       <c r="E8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="5" t="s">
+      <c r="F8" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="9" t="s">
         <v>26</v>
       </c>
       <c r="H8" s="5" t="s">
@@ -1060,7 +1060,7 @@
       <c r="A9" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -1072,10 +1072,10 @@
       <c r="E9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="5" t="s">
+      <c r="F9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="8" t="s">
         <v>26</v>
       </c>
       <c r="H9" s="5" t="s">
@@ -1206,7 +1206,7 @@
       <c r="A11" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -1271,7 +1271,7 @@
       <c r="X11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="Y11" s="9" t="s">
+      <c r="Y11" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1279,7 +1279,7 @@
       <c r="A12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C12" s="5" t="s">
@@ -1344,7 +1344,7 @@
       <c r="X12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="Y12" s="9" t="s">
+      <c r="Y12" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1352,7 +1352,7 @@
       <c r="A13" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="5" t="s">
@@ -1417,7 +1417,7 @@
       <c r="X13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="Y13" s="8" t="s">
+      <c r="Y13" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1519,7 +1519,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+      <selection pane="topLeft" activeCell="D19" activeCellId="1" sqref="F8:G8 D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1576,7 +1576,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
+      <selection pane="topLeft" activeCell="B34" activeCellId="1" sqref="F8:G8 B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1633,7 +1633,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="F8:G8 A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1682,7 +1682,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="1" sqref="F8:G8 B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1843,7 +1843,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="F8:G8 B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Fixed regressopns (#245, #246)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -380,11 +380,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -480,7 +480,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F8" activeCellId="0" sqref="F8:G8"/>
+      <selection pane="bottomRight" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -822,7 +822,7 @@
       <c r="S5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="T5" s="8" t="s">
+      <c r="T5" s="9" t="s">
         <v>27</v>
       </c>
       <c r="U5" s="5" t="s">
@@ -895,7 +895,7 @@
       <c r="S6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="T6" s="8" t="s">
+      <c r="T6" s="9" t="s">
         <v>27</v>
       </c>
       <c r="U6" s="5" t="s">
@@ -932,7 +932,7 @@
       <c r="G7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="9" t="s">
         <v>26</v>
       </c>
       <c r="I7" s="5" t="s">
@@ -951,7 +951,7 @@
         <v>26</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O7" s="5" t="s">
         <v>26</v>
@@ -999,10 +999,10 @@
       <c r="E8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="9" t="s">
+      <c r="F8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>26</v>
       </c>
       <c r="H8" s="5" t="s">
@@ -1011,7 +1011,7 @@
       <c r="I8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="J8" s="9" t="s">
         <v>26</v>
       </c>
       <c r="K8" s="5" t="s">
@@ -1035,13 +1035,13 @@
       <c r="Q8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="R8" s="8" t="s">
+      <c r="R8" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="T8" s="8" t="s">
+      <c r="T8" s="9" t="s">
         <v>27</v>
       </c>
       <c r="U8" s="5" t="s">
@@ -1049,7 +1049,7 @@
       </c>
       <c r="V8" s="7"/>
       <c r="W8" s="7"/>
-      <c r="X8" s="8" t="s">
+      <c r="X8" s="9" t="s">
         <v>26</v>
       </c>
       <c r="Y8" s="5" t="s">
@@ -1105,16 +1105,16 @@
       <c r="P9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="Q9" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="R9" s="8" t="s">
+      <c r="Q9" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="R9" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="T9" s="8" t="s">
+      <c r="T9" s="9" t="s">
         <v>27</v>
       </c>
       <c r="U9" s="5" t="s">
@@ -1133,7 +1133,7 @@
       <c r="A10" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="9" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -1151,7 +1151,7 @@
       <c r="G10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="9" t="s">
         <v>26</v>
       </c>
       <c r="I10" s="5" t="s">
@@ -1160,13 +1160,13 @@
       <c r="J10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K10" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="M10" s="8" t="s">
+      <c r="K10" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="M10" s="9" t="s">
         <v>27</v>
       </c>
       <c r="N10" s="5" t="s">
@@ -1184,7 +1184,7 @@
       <c r="R10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="S10" s="8" t="s">
+      <c r="S10" s="9" t="s">
         <v>26</v>
       </c>
       <c r="T10" s="5" t="s">
@@ -1198,7 +1198,7 @@
       <c r="X10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="Y10" s="8" t="s">
+      <c r="Y10" s="9" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1240,7 +1240,7 @@
         <v>26</v>
       </c>
       <c r="M11" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N11" s="5" t="s">
         <v>27</v>
@@ -1324,7 +1324,7 @@
       <c r="P12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="Q12" s="8" t="s">
+      <c r="Q12" s="9" t="s">
         <v>26</v>
       </c>
       <c r="R12" s="5" t="s">
@@ -1394,7 +1394,7 @@
       <c r="O13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="P13" s="8" t="s">
+      <c r="P13" s="9" t="s">
         <v>26</v>
       </c>
       <c r="Q13" s="5" t="s">
@@ -1519,7 +1519,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="1" sqref="F8:G8 D19"/>
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1576,7 +1576,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B34" activeCellId="1" sqref="F8:G8 B34"/>
+      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1633,7 +1633,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="F8:G8 A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1682,7 +1682,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="1" sqref="F8:G8 B17"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1843,7 +1843,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="F8:G8 B6"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Error when comptime types are found in bare unions (#248)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -380,11 +380,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -480,7 +480,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H11" activeCellId="0" sqref="H11"/>
+      <selection pane="bottomRight" activeCell="Q12" activeCellId="0" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -687,7 +687,7 @@
       <c r="X3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="Y3" s="8" t="s">
+      <c r="Y3" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -822,7 +822,7 @@
       <c r="S5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="T5" s="9" t="s">
+      <c r="T5" s="8" t="s">
         <v>27</v>
       </c>
       <c r="U5" s="5" t="s">
@@ -895,7 +895,7 @@
       <c r="S6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="T6" s="9" t="s">
+      <c r="T6" s="8" t="s">
         <v>27</v>
       </c>
       <c r="U6" s="5" t="s">
@@ -932,7 +932,7 @@
       <c r="G7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I7" s="5" t="s">
@@ -947,7 +947,7 @@
       <c r="L7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="M7" s="8" t="s">
+      <c r="M7" s="5" t="s">
         <v>26</v>
       </c>
       <c r="N7" s="5" t="s">
@@ -1011,7 +1011,7 @@
       <c r="I8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="J8" s="8" t="s">
         <v>26</v>
       </c>
       <c r="K8" s="5" t="s">
@@ -1035,13 +1035,13 @@
       <c r="Q8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="R8" s="9" t="s">
+      <c r="R8" s="8" t="s">
         <v>26</v>
       </c>
       <c r="S8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="T8" s="9" t="s">
+      <c r="T8" s="8" t="s">
         <v>27</v>
       </c>
       <c r="U8" s="5" t="s">
@@ -1049,7 +1049,7 @@
       </c>
       <c r="V8" s="7"/>
       <c r="W8" s="7"/>
-      <c r="X8" s="9" t="s">
+      <c r="X8" s="8" t="s">
         <v>26</v>
       </c>
       <c r="Y8" s="5" t="s">
@@ -1060,7 +1060,7 @@
       <c r="A9" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -1072,10 +1072,10 @@
       <c r="E9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="8" t="s">
+      <c r="F9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>26</v>
       </c>
       <c r="H9" s="5" t="s">
@@ -1093,7 +1093,7 @@
       <c r="L9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="M9" s="8" t="s">
+      <c r="M9" s="5" t="s">
         <v>26</v>
       </c>
       <c r="N9" s="5" t="s">
@@ -1105,16 +1105,16 @@
       <c r="P9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="Q9" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="R9" s="9" t="s">
+      <c r="Q9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="R9" s="8" t="s">
         <v>26</v>
       </c>
       <c r="S9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="T9" s="9" t="s">
+      <c r="T9" s="8" t="s">
         <v>27</v>
       </c>
       <c r="U9" s="5" t="s">
@@ -1134,7 +1134,7 @@
         <v>34</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>26</v>
@@ -1151,7 +1151,7 @@
       <c r="G10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H10" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I10" s="5" t="s">
@@ -1161,10 +1161,10 @@
         <v>26</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L10" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M10" s="9" t="s">
         <v>27</v>
@@ -1184,7 +1184,7 @@
       <c r="R10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="S10" s="9" t="s">
+      <c r="S10" s="8" t="s">
         <v>26</v>
       </c>
       <c r="T10" s="5" t="s">
@@ -1199,7 +1199,7 @@
         <v>26</v>
       </c>
       <c r="Y10" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1239,7 +1239,7 @@
       <c r="L11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="M11" s="8" t="s">
+      <c r="M11" s="5" t="s">
         <v>26</v>
       </c>
       <c r="N11" s="5" t="s">
@@ -1324,7 +1324,7 @@
       <c r="P12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="Q12" s="9" t="s">
+      <c r="Q12" s="8" t="s">
         <v>26</v>
       </c>
       <c r="R12" s="5" t="s">
@@ -1394,7 +1394,7 @@
       <c r="O13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="P13" s="9" t="s">
+      <c r="P13" s="8" t="s">
         <v>26</v>
       </c>
       <c r="Q13" s="5" t="s">

</xml_diff>

<commit_message>
Fixed regressions (#249, #250, #251)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -372,6 +372,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -381,10 +385,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -480,7 +480,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Q12" activeCellId="0" sqref="Q12"/>
+      <selection pane="bottomRight" activeCell="Q14" activeCellId="0" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -664,7 +664,7 @@
       <c r="O3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="P3" s="6" t="s">
         <v>26</v>
       </c>
       <c r="Q3" s="5" t="s">
@@ -673,7 +673,7 @@
       <c r="R3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="S3" s="7" t="s">
         <v>26</v>
       </c>
       <c r="T3" s="5" t="s">
@@ -682,8 +682,8 @@
       <c r="U3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="V3" s="7"/>
-      <c r="W3" s="7"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
       <c r="X3" s="5" t="s">
         <v>26</v>
       </c>
@@ -755,8 +755,8 @@
       <c r="U4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="V4" s="7"/>
-      <c r="W4" s="7"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
       <c r="X4" s="5" t="s">
         <v>26</v>
       </c>
@@ -822,14 +822,14 @@
       <c r="S5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="T5" s="8" t="s">
+      <c r="T5" s="9" t="s">
         <v>27</v>
       </c>
       <c r="U5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="V5" s="7"/>
-      <c r="W5" s="7"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
       <c r="X5" s="5" t="s">
         <v>26</v>
       </c>
@@ -880,10 +880,10 @@
       <c r="N6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="O6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="P6" s="5" t="s">
+      <c r="O6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="P6" s="6" t="s">
         <v>26</v>
       </c>
       <c r="Q6" s="5" t="s">
@@ -895,14 +895,14 @@
       <c r="S6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="T6" s="8" t="s">
+      <c r="T6" s="9" t="s">
         <v>27</v>
       </c>
       <c r="U6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="V6" s="7"/>
-      <c r="W6" s="7"/>
+      <c r="V6" s="8"/>
+      <c r="W6" s="8"/>
       <c r="X6" s="5" t="s">
         <v>26</v>
       </c>
@@ -932,7 +932,7 @@
       <c r="G7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="9" t="s">
         <v>26</v>
       </c>
       <c r="I7" s="5" t="s">
@@ -953,10 +953,10 @@
       <c r="N7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="O7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="P7" s="5" t="s">
+      <c r="O7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="P7" s="6" t="s">
         <v>26</v>
       </c>
       <c r="Q7" s="5" t="s">
@@ -974,8 +974,8 @@
       <c r="U7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="V7" s="7"/>
-      <c r="W7" s="7"/>
+      <c r="V7" s="8"/>
+      <c r="W7" s="8"/>
       <c r="X7" s="5" t="s">
         <v>26</v>
       </c>
@@ -1011,7 +1011,7 @@
       <c r="I8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="J8" s="9" t="s">
         <v>26</v>
       </c>
       <c r="K8" s="5" t="s">
@@ -1030,26 +1030,26 @@
         <v>26</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="R8" s="8" t="s">
+      <c r="R8" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="T8" s="8" t="s">
+      <c r="T8" s="9" t="s">
         <v>27</v>
       </c>
       <c r="U8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="V8" s="7"/>
-      <c r="W8" s="7"/>
-      <c r="X8" s="8" t="s">
+      <c r="V8" s="8"/>
+      <c r="W8" s="8"/>
+      <c r="X8" s="9" t="s">
         <v>26</v>
       </c>
       <c r="Y8" s="5" t="s">
@@ -1105,23 +1105,23 @@
       <c r="P9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="Q9" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="R9" s="8" t="s">
+      <c r="Q9" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="R9" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="T9" s="8" t="s">
+      <c r="T9" s="9" t="s">
         <v>27</v>
       </c>
       <c r="U9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="V9" s="7"/>
-      <c r="W9" s="7"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="8"/>
       <c r="X9" s="5" t="s">
         <v>26</v>
       </c>
@@ -1133,7 +1133,7 @@
       <c r="A10" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -1151,7 +1151,7 @@
       <c r="G10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="9" t="s">
         <v>26</v>
       </c>
       <c r="I10" s="5" t="s">
@@ -1160,13 +1160,13 @@
       <c r="J10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K10" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="L10" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="M10" s="9" t="s">
+      <c r="K10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M10" s="5" t="s">
         <v>27</v>
       </c>
       <c r="N10" s="5" t="s">
@@ -1184,7 +1184,7 @@
       <c r="R10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="S10" s="8" t="s">
+      <c r="S10" s="9" t="s">
         <v>26</v>
       </c>
       <c r="T10" s="5" t="s">
@@ -1193,12 +1193,12 @@
       <c r="U10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="V10" s="7"/>
-      <c r="W10" s="7"/>
+      <c r="V10" s="8"/>
+      <c r="W10" s="8"/>
       <c r="X10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="Y10" s="9" t="s">
+      <c r="Y10" s="5" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1266,8 +1266,8 @@
       <c r="U11" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="V11" s="7"/>
-      <c r="W11" s="7"/>
+      <c r="V11" s="8"/>
+      <c r="W11" s="8"/>
       <c r="X11" s="5" t="s">
         <v>26</v>
       </c>
@@ -1324,7 +1324,7 @@
       <c r="P12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="Q12" s="8" t="s">
+      <c r="Q12" s="9" t="s">
         <v>26</v>
       </c>
       <c r="R12" s="5" t="s">
@@ -1339,8 +1339,8 @@
       <c r="U12" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="V12" s="7"/>
-      <c r="W12" s="7"/>
+      <c r="V12" s="8"/>
+      <c r="W12" s="8"/>
       <c r="X12" s="5" t="s">
         <v>26</v>
       </c>
@@ -1394,7 +1394,7 @@
       <c r="O13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="P13" s="8" t="s">
+      <c r="P13" s="9" t="s">
         <v>26</v>
       </c>
       <c r="Q13" s="5" t="s">
@@ -1412,8 +1412,8 @@
       <c r="U13" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="V13" s="7"/>
-      <c r="W13" s="7"/>
+      <c r="V13" s="8"/>
+      <c r="W13" s="8"/>
       <c r="X13" s="5" t="s">
         <v>26</v>
       </c>
@@ -1485,8 +1485,8 @@
       <c r="U14" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="V14" s="7"/>
-      <c r="W14" s="7"/>
+      <c r="V14" s="8"/>
+      <c r="W14" s="8"/>
       <c r="X14" s="5" t="s">
         <v>27</v>
       </c>
@@ -1682,7 +1682,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1720,7 +1720,7 @@
       <c r="A5" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="9" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1728,7 +1728,7 @@
       <c r="A6" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="9" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1768,7 +1768,7 @@
       <c r="A11" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="9" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1784,7 +1784,7 @@
       <c r="A13" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="9" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed handling of functions (#252)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -372,15 +372,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -480,7 +480,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Q14" activeCellId="0" sqref="Q14"/>
+      <selection pane="bottomRight" activeCell="P9" activeCellId="0" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -664,7 +664,7 @@
       <c r="O3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="P3" s="5" t="s">
         <v>26</v>
       </c>
       <c r="Q3" s="5" t="s">
@@ -673,7 +673,7 @@
       <c r="R3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="S3" s="7" t="s">
+      <c r="S3" s="6" t="s">
         <v>26</v>
       </c>
       <c r="T3" s="5" t="s">
@@ -682,8 +682,8 @@
       <c r="U3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
       <c r="X3" s="5" t="s">
         <v>26</v>
       </c>
@@ -755,8 +755,8 @@
       <c r="U4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="V4" s="8"/>
-      <c r="W4" s="8"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
       <c r="X4" s="5" t="s">
         <v>26</v>
       </c>
@@ -822,14 +822,14 @@
       <c r="S5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="T5" s="9" t="s">
+      <c r="T5" s="8" t="s">
         <v>27</v>
       </c>
       <c r="U5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="V5" s="8"/>
-      <c r="W5" s="8"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="7"/>
       <c r="X5" s="5" t="s">
         <v>26</v>
       </c>
@@ -880,10 +880,10 @@
       <c r="N6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="O6" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="P6" s="6" t="s">
+      <c r="O6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="P6" s="5" t="s">
         <v>26</v>
       </c>
       <c r="Q6" s="5" t="s">
@@ -895,14 +895,14 @@
       <c r="S6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="T6" s="9" t="s">
+      <c r="T6" s="8" t="s">
         <v>27</v>
       </c>
       <c r="U6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="V6" s="8"/>
-      <c r="W6" s="8"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
       <c r="X6" s="5" t="s">
         <v>26</v>
       </c>
@@ -953,10 +953,10 @@
       <c r="N7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="O7" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="P7" s="6" t="s">
+      <c r="O7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="P7" s="5" t="s">
         <v>26</v>
       </c>
       <c r="Q7" s="5" t="s">
@@ -974,8 +974,8 @@
       <c r="U7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="V7" s="8"/>
-      <c r="W7" s="8"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
       <c r="X7" s="5" t="s">
         <v>26</v>
       </c>
@@ -1041,14 +1041,14 @@
       <c r="S8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="T8" s="9" t="s">
+      <c r="T8" s="8" t="s">
         <v>27</v>
       </c>
       <c r="U8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="V8" s="8"/>
-      <c r="W8" s="8"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="7"/>
       <c r="X8" s="9" t="s">
         <v>26</v>
       </c>
@@ -1114,14 +1114,14 @@
       <c r="S9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="T9" s="9" t="s">
+      <c r="T9" s="8" t="s">
         <v>27</v>
       </c>
       <c r="U9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="V9" s="8"/>
-      <c r="W9" s="8"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
       <c r="X9" s="5" t="s">
         <v>26</v>
       </c>
@@ -1193,8 +1193,8 @@
       <c r="U10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="V10" s="8"/>
-      <c r="W10" s="8"/>
+      <c r="V10" s="7"/>
+      <c r="W10" s="7"/>
       <c r="X10" s="5" t="s">
         <v>26</v>
       </c>
@@ -1266,8 +1266,8 @@
       <c r="U11" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="V11" s="8"/>
-      <c r="W11" s="8"/>
+      <c r="V11" s="7"/>
+      <c r="W11" s="7"/>
       <c r="X11" s="5" t="s">
         <v>26</v>
       </c>
@@ -1339,8 +1339,8 @@
       <c r="U12" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="V12" s="8"/>
-      <c r="W12" s="8"/>
+      <c r="V12" s="7"/>
+      <c r="W12" s="7"/>
       <c r="X12" s="5" t="s">
         <v>26</v>
       </c>
@@ -1412,8 +1412,8 @@
       <c r="U13" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="V13" s="8"/>
-      <c r="W13" s="8"/>
+      <c r="V13" s="7"/>
+      <c r="W13" s="7"/>
       <c r="X13" s="5" t="s">
         <v>26</v>
       </c>
@@ -1485,8 +1485,8 @@
       <c r="U14" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="V14" s="8"/>
-      <c r="W14" s="8"/>
+      <c r="V14" s="7"/>
+      <c r="W14" s="7"/>
       <c r="X14" s="5" t="s">
         <v>27</v>
       </c>
@@ -1682,7 +1682,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1720,7 +1720,7 @@
       <c r="A5" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1728,7 +1728,7 @@
       <c r="A6" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1768,7 +1768,7 @@
       <c r="A11" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1784,7 +1784,7 @@
       <c r="A13" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="5" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed various regressions (#264)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -388,7 +388,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -480,7 +480,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="P9" activeCellId="0" sqref="P9"/>
+      <selection pane="bottomRight" activeCell="P14" activeCellId="0" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -822,7 +822,7 @@
       <c r="S5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="T5" s="8" t="s">
+      <c r="T5" s="5" t="s">
         <v>27</v>
       </c>
       <c r="U5" s="5" t="s">
@@ -895,7 +895,7 @@
       <c r="S6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="T6" s="8" t="s">
+      <c r="T6" s="5" t="s">
         <v>27</v>
       </c>
       <c r="U6" s="5" t="s">
@@ -932,7 +932,7 @@
       <c r="G7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I7" s="5" t="s">
@@ -1041,7 +1041,7 @@
       <c r="S8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="T8" s="8" t="s">
+      <c r="T8" s="5" t="s">
         <v>27</v>
       </c>
       <c r="U8" s="5" t="s">
@@ -1114,7 +1114,7 @@
       <c r="S9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="T9" s="8" t="s">
+      <c r="T9" s="5" t="s">
         <v>27</v>
       </c>
       <c r="U9" s="5" t="s">
@@ -1152,7 +1152,7 @@
         <v>26</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Reworked enum and error set (#264)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -480,7 +480,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="T9" activeCellId="0" sqref="T9"/>
+      <selection pane="bottomRight" activeCell="Q10" activeCellId="0" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -915,7 +915,7 @@
         <v>31</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>26</v>
@@ -1035,7 +1035,7 @@
       <c r="Q8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="R8" s="8" t="s">
+      <c r="R8" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S8" s="5" t="s">
@@ -1105,10 +1105,10 @@
       <c r="P9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="Q9" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="R9" s="9" t="s">
+      <c r="Q9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="R9" s="5" t="s">
         <v>26</v>
       </c>
       <c r="S9" s="5" t="s">
@@ -1324,7 +1324,7 @@
       <c r="P12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="Q12" s="9" t="s">
+      <c r="Q12" s="5" t="s">
         <v>26</v>
       </c>
       <c r="R12" s="5" t="s">
@@ -1394,7 +1394,7 @@
       <c r="O13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="P13" s="8" t="s">
+      <c r="P13" s="9" t="s">
         <v>26</v>
       </c>
       <c r="Q13" s="5" t="s">

</xml_diff>

<commit_message>
Fixed issues related to default values (#264)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -380,11 +380,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -480,7 +480,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Q10" activeCellId="0" sqref="Q10"/>
+      <selection pane="bottomRight" activeCell="X8" activeCellId="0" sqref="X8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1011,7 +1011,7 @@
       <c r="I8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="J8" s="9" t="s">
         <v>26</v>
       </c>
       <c r="K8" s="5" t="s">
@@ -1035,7 +1035,7 @@
       <c r="Q8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="R8" s="9" t="s">
+      <c r="R8" s="5" t="s">
         <v>26</v>
       </c>
       <c r="S8" s="5" t="s">
@@ -1049,7 +1049,7 @@
       </c>
       <c r="V8" s="7"/>
       <c r="W8" s="7"/>
-      <c r="X8" s="8" t="s">
+      <c r="X8" s="9" t="s">
         <v>26</v>
       </c>
       <c r="Y8" s="5" t="s">
@@ -1114,7 +1114,7 @@
       <c r="S9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="T9" s="8" t="s">
+      <c r="T9" s="9" t="s">
         <v>27</v>
       </c>
       <c r="U9" s="5" t="s">
@@ -1151,7 +1151,7 @@
       <c r="G10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="9" t="s">
         <v>27</v>
       </c>
       <c r="I10" s="5" t="s">
@@ -1184,7 +1184,7 @@
       <c r="R10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="S10" s="8" t="s">
+      <c r="S10" s="9" t="s">
         <v>26</v>
       </c>
       <c r="T10" s="5" t="s">
@@ -1394,7 +1394,7 @@
       <c r="O13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="P13" s="9" t="s">
+      <c r="P13" s="5" t="s">
         <v>26</v>
       </c>
       <c r="Q13" s="5" t="s">

</xml_diff>

<commit_message>
Fixed regression with function handling (#264)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -380,11 +380,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -480,7 +480,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="X8" activeCellId="0" sqref="X8"/>
+      <selection pane="bottomRight" activeCell="M14" activeCellId="0" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -938,7 +938,7 @@
       <c r="I7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="J7" s="5" t="s">
         <v>26</v>
       </c>
       <c r="K7" s="5" t="s">
@@ -965,7 +965,7 @@
       <c r="R7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="S7" s="8" t="s">
+      <c r="S7" s="5" t="s">
         <v>26</v>
       </c>
       <c r="T7" s="5" t="s">
@@ -1011,7 +1011,7 @@
       <c r="I8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="J8" s="8" t="s">
         <v>26</v>
       </c>
       <c r="K8" s="5" t="s">
@@ -1049,7 +1049,7 @@
       </c>
       <c r="V8" s="7"/>
       <c r="W8" s="7"/>
-      <c r="X8" s="9" t="s">
+      <c r="X8" s="8" t="s">
         <v>26</v>
       </c>
       <c r="Y8" s="5" t="s">
@@ -1151,7 +1151,7 @@
       <c r="G10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H10" s="8" t="s">
         <v>27</v>
       </c>
       <c r="I10" s="5" t="s">
@@ -1184,7 +1184,7 @@
       <c r="R10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="S10" s="9" t="s">
+      <c r="S10" s="8" t="s">
         <v>26</v>
       </c>
       <c r="T10" s="5" t="s">

</xml_diff>

<commit_message>
Implemented handling of struct in packed struct (#264)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -380,11 +380,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -480,7 +480,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M14" activeCellId="0" sqref="M14"/>
+      <selection pane="bottomRight" activeCell="K12" activeCellId="0" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1012,7 +1012,7 @@
         <v>27</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K8" s="5" t="s">
         <v>26</v>
@@ -1050,7 +1050,7 @@
       <c r="V8" s="7"/>
       <c r="W8" s="7"/>
       <c r="X8" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Y8" s="5" t="s">
         <v>27</v>
@@ -1114,7 +1114,7 @@
       <c r="S9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="T9" s="9" t="s">
+      <c r="T9" s="5" t="s">
         <v>27</v>
       </c>
       <c r="U9" s="5" t="s">
@@ -1151,7 +1151,7 @@
       <c r="G10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="9" t="s">
         <v>27</v>
       </c>
       <c r="I10" s="5" t="s">
@@ -1184,7 +1184,7 @@
       <c r="R10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="S10" s="8" t="s">
+      <c r="S10" s="9" t="s">
         <v>26</v>
       </c>
       <c r="T10" s="5" t="s">

</xml_diff>

<commit_message>
Fixed pointer in bare union (#264)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -480,7 +480,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K12" activeCellId="0" sqref="K12"/>
+      <selection pane="bottomRight" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1011,7 +1011,7 @@
       <c r="I8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="J8" s="5" t="s">
         <v>27</v>
       </c>
       <c r="K8" s="5" t="s">
@@ -1049,7 +1049,7 @@
       </c>
       <c r="V8" s="7"/>
       <c r="W8" s="7"/>
-      <c r="X8" s="8" t="s">
+      <c r="X8" s="5" t="s">
         <v>27</v>
       </c>
       <c r="Y8" s="5" t="s">
@@ -1151,7 +1151,7 @@
       <c r="G10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H10" s="8" t="s">
         <v>27</v>
       </c>
       <c r="I10" s="5" t="s">

</xml_diff>

<commit_message>
Implemented target updating (#262)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="64">
   <si>
     <t xml:space="preserve">Context</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t xml:space="preserve">Allow call as methods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change pointer target</t>
   </si>
   <si>
     <t xml:space="preserve">Create internal slice</t>
@@ -341,7 +344,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -371,10 +374,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1174,7 +1173,7 @@
       <c r="R10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="S10" s="8" t="s">
+      <c r="S10" s="5" t="s">
         <v>26</v>
       </c>
       <c r="T10" s="5" t="s">
@@ -1214,7 +1213,7 @@
       <c r="G11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H11" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I11" s="5" t="s">
@@ -1521,11 +1520,11 @@
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="10"/>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="10"/>
+      <c r="B2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -1578,11 +1577,11 @@
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="10"/>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="10"/>
+      <c r="B2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -1635,11 +1634,11 @@
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="10"/>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="10"/>
+      <c r="B2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -1669,13 +1668,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.06"/>
   </cols>
@@ -1684,11 +1683,11 @@
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="10"/>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="10"/>
+      <c r="B2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -1807,6 +1806,14 @@
         <v>59</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1845,15 +1852,15 @@
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="10"/>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="10"/>
+      <c r="B2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>26</v>
@@ -1861,7 +1868,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>26</v>
@@ -1869,7 +1876,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Added checks for valueOf() and toJSON() (#258)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -10,7 +10,7 @@
   <sheets>
     <sheet name="Type handling" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Console" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Crypto" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Built-in functions" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Error handling" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Function calling" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Memory allocation" sheetId="6" state="visible" r:id="rId7"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="69">
   <si>
     <t xml:space="preserve">Context</t>
   </si>
@@ -157,6 +157,21 @@
   </si>
   <si>
     <t xml:space="preserve">Generate sha1 hash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generate CityHash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uncompress gzip data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uncompress xz data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generate random numbers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Return total system memory</t>
   </si>
   <si>
     <t xml:space="preserve">WASM error trace</t>
@@ -1562,10 +1577,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1597,6 +1612,32 @@
       </c>
       <c r="B4" s="5" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="5"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1642,7 +1683,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>26</v>
@@ -1691,7 +1732,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>26</v>
@@ -1699,7 +1740,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>26</v>
@@ -1707,7 +1748,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>26</v>
@@ -1715,7 +1756,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>26</v>
@@ -1723,7 +1764,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>26</v>
@@ -1731,7 +1772,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>26</v>
@@ -1739,7 +1780,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>26</v>
@@ -1747,7 +1788,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>26</v>
@@ -1755,7 +1796,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>26</v>
@@ -1763,7 +1804,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>26</v>
@@ -1771,7 +1812,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>26</v>
@@ -1779,7 +1820,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>26</v>
@@ -1787,7 +1828,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>26</v>
@@ -1795,7 +1836,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>26</v>
@@ -1803,7 +1844,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>26</v>
@@ -1811,7 +1852,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>26</v>
@@ -1860,7 +1901,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>26</v>
@@ -1868,7 +1909,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>26</v>
@@ -1876,7 +1917,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Allow build.zig to work in both 0.11.0 and 0.12.0 (#272)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -14,6 +14,7 @@
     <sheet name="Error handling" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Function calling" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Memory allocation" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Package manager" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="71">
   <si>
     <t xml:space="preserve">Context</t>
   </si>
@@ -232,6 +233,12 @@
   </si>
   <si>
     <t xml:space="preserve">Create fixed object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using ziglua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using zig-sqlite</t>
   </si>
 </sst>
 </file>
@@ -1936,4 +1943,61 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="9"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="9"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="5"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="5"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added package manager tests (#253, #272)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Type handling" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="72">
   <si>
     <t xml:space="preserve">Context</t>
   </si>
@@ -239,6 +239,9 @@
   </si>
   <si>
     <t xml:space="preserve">Using zig-sqlite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using zigplotlib</t>
   </si>
 </sst>
 </file>
@@ -486,7 +489,7 @@
   </sheetPr>
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -1952,7 +1955,7 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -1975,17 +1978,25 @@
       <c r="A3" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
+      <c r="A5" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Added test for ziglyph (#253)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Type handling" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="73">
   <si>
     <t xml:space="preserve">Context</t>
   </si>
@@ -242,6 +242,9 @@
   </si>
   <si>
     <t xml:space="preserve">Using zigplotlib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using ziglyph</t>
   </si>
 </sst>
 </file>
@@ -489,7 +492,7 @@
   </sheetPr>
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -1953,10 +1956,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1995,6 +1998,14 @@
         <v>71</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed opaque pointer handling (#275)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Type handling" sheetId="1" state="visible" r:id="rId2"/>
@@ -495,12 +495,12 @@
   </sheetPr>
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="S10" activeCellId="0" sqref="S10"/>
+      <selection pane="bottomRight" activeCell="H15" activeCellId="0" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -700,7 +700,7 @@
         <v>27</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V3" s="7"/>
       <c r="W3" s="7"/>
@@ -773,7 +773,7 @@
         <v>27</v>
       </c>
       <c r="U4" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V4" s="7"/>
       <c r="W4" s="7"/>
@@ -846,7 +846,7 @@
         <v>27</v>
       </c>
       <c r="U5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V5" s="7"/>
       <c r="W5" s="7"/>
@@ -919,7 +919,7 @@
         <v>27</v>
       </c>
       <c r="U6" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V6" s="7"/>
       <c r="W6" s="7"/>
@@ -992,7 +992,7 @@
         <v>27</v>
       </c>
       <c r="U7" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V7" s="7"/>
       <c r="W7" s="7"/>
@@ -1138,7 +1138,7 @@
         <v>27</v>
       </c>
       <c r="U9" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V9" s="7"/>
       <c r="W9" s="7"/>
@@ -1284,7 +1284,7 @@
         <v>27</v>
       </c>
       <c r="U11" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V11" s="7"/>
       <c r="W11" s="7"/>
@@ -1357,7 +1357,7 @@
         <v>27</v>
       </c>
       <c r="U12" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V12" s="7"/>
       <c r="W12" s="7"/>
@@ -1430,7 +1430,7 @@
         <v>27</v>
       </c>
       <c r="U13" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V13" s="7"/>
       <c r="W13" s="7"/>
@@ -1464,7 +1464,7 @@
         <v>26</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I14" s="5" t="s">
         <v>27</v>
@@ -1961,7 +1961,7 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed exporter issues (#340)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="75">
   <si>
     <t xml:space="preserve">Context</t>
   </si>
@@ -224,6 +224,9 @@
   </si>
   <si>
     <t xml:space="preserve">Change pointer target</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inline function</t>
   </si>
   <si>
     <t xml:space="preserve">Create internal slice</t>
@@ -500,7 +503,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H15" activeCellId="0" sqref="H15"/>
+      <selection pane="bottomRight" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1725,10 +1728,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1871,6 +1874,14 @@
         <v>65</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1917,7 +1928,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>26</v>
@@ -1925,7 +1936,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>26</v>
@@ -1933,7 +1944,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>26</v>
@@ -1982,7 +1993,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>26</v>
@@ -1990,7 +2001,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>26</v>
@@ -1998,7 +2009,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>26</v>
@@ -2006,7 +2017,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>26</v>
@@ -2014,7 +2025,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B7" s="5"/>
     </row>

</xml_diff>

<commit_message>
Adjusted const implementation (#341)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Type handling" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="77">
   <si>
     <t xml:space="preserve">Context</t>
   </si>
@@ -230,6 +230,9 @@
   </si>
   <si>
     <t xml:space="preserve">Handle pointers in struct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Return const pointer</t>
   </si>
   <si>
     <t xml:space="preserve">Create internal slice</t>
@@ -501,7 +504,7 @@
   </sheetPr>
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
@@ -1731,10 +1734,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1893,7 +1896,15 @@
         <v>67</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1939,7 +1950,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>26</v>
@@ -1947,7 +1958,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>26</v>
@@ -1955,7 +1966,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>26</v>
@@ -2004,7 +2015,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>26</v>
@@ -2012,7 +2023,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>26</v>
@@ -2020,7 +2031,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>26</v>
@@ -2028,7 +2039,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>26</v>
@@ -2036,7 +2047,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B7" s="5"/>
     </row>

</xml_diff>

<commit_message>
Fixed arg struct name issue (#361)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="79">
   <si>
     <t xml:space="preserve">Context</t>
   </si>
@@ -179,6 +179,9 @@
   </si>
   <si>
     <t xml:space="preserve">Throw error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Throw error when arguments are off</t>
   </si>
   <si>
     <t xml:space="preserve">Return slice</t>
@@ -387,7 +390,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -425,10 +428,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -516,7 +515,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H3" activeCellId="0" sqref="H3"/>
+      <selection pane="bottomRight" activeCell="N11" activeCellId="0" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1741,10 +1740,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1910,7 +1909,7 @@
       <c r="A21" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1919,6 +1918,14 @@
         <v>69</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1965,7 +1972,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>26</v>
@@ -1973,7 +1980,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>26</v>
@@ -1981,7 +1988,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>26</v>
@@ -2030,7 +2037,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>26</v>
@@ -2038,7 +2045,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>26</v>
@@ -2046,7 +2053,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>26</v>
@@ -2054,7 +2061,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>26</v>
@@ -2062,7 +2069,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B7" s="5"/>
     </row>

</xml_diff>

<commit_message>
Began implementing iterator support (#387)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Type handling" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,6 +15,7 @@
     <sheet name="Function calling" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Memory allocation" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="Package manager" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Iterator" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="83">
   <si>
     <t xml:space="preserve">Context</t>
   </si>
@@ -263,6 +264,18 @@
   </si>
   <si>
     <t xml:space="preserve">Using zig-duckdb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">std.mem.SplitIterator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">std.zig.Iterator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">std.fs.Dir.Iterator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">std.fs.path.ComponentIterator</t>
   </si>
 </sst>
 </file>
@@ -510,7 +523,7 @@
   </sheetPr>
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
@@ -2086,4 +2099,70 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="9"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="9"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="5"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="5"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="5"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="5"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added iterator test (#387)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="83">
   <si>
     <t xml:space="preserve">Context</t>
   </si>
@@ -2109,7 +2109,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2131,7 +2131,9 @@
       <c r="A3" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">

</xml_diff>

<commit_message>
Added more iterator tests (#387)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="83">
   <si>
     <t xml:space="preserve">Context</t>
   </si>
@@ -269,7 +269,7 @@
     <t xml:space="preserve">std.mem.SplitIterator</t>
   </si>
   <si>
-    <t xml:space="preserve">std.zig.Iterator</t>
+    <t xml:space="preserve">std.zip.Iterator</t>
   </si>
   <si>
     <t xml:space="preserve">std.fs.Dir.Iterator</t>
@@ -2109,7 +2109,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2139,19 +2139,25 @@
       <c r="A4" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B4" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B6" s="5"/>
+      <c r="B6" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>

<commit_message>
Added test case (#448)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="89">
   <si>
     <t xml:space="preserve">Context</t>
   </si>
@@ -547,7 +547,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N11" activeCellId="0" sqref="N11"/>
+      <selection pane="bottomRight" activeCell="N11" activeCellId="1" sqref="B7:B8 N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1586,7 +1586,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+      <selection pane="topLeft" activeCell="D19" activeCellId="1" sqref="B7:B8 D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1643,7 +1643,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="1" sqref="B7:B8 C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1726,7 +1726,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="B7:B8 A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1775,7 +1775,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="1" sqref="B7:B8 B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1984,7 +1984,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="B7:B8 B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2049,7 +2049,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2071,35 +2071,48 @@
       <c r="A3" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B6" s="5"/>
+      <c r="B6" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B7" s="5"/>
+      <c r="B7" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
         <v>79</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -2125,7 +2138,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B7:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2204,7 +2217,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I41" activeCellId="0" sqref="I41"/>
+      <selection pane="topLeft" activeCell="I41" activeCellId="1" sqref="B7:B8 I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Implemented releasing of context (#454)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Type handling" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="90">
   <si>
     <t xml:space="preserve">Context</t>
   </si>
@@ -249,7 +249,10 @@
     <t xml:space="preserve">Allocate memory for string</t>
   </si>
   <si>
-    <t xml:space="preserve">Create fixed object</t>
+    <t xml:space="preserve">Retain allocator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Return allocator</t>
   </si>
   <si>
     <t xml:space="preserve">Thread creation</t>
@@ -547,7 +550,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N11" activeCellId="1" sqref="B7:B8 N11"/>
+      <selection pane="bottomRight" activeCell="N11" activeCellId="0" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1586,7 +1589,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="1" sqref="B7:B8 D19"/>
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1643,7 +1646,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="1" sqref="B7:B8 C10"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1726,7 +1729,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="B7:B8 A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1775,7 +1778,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="1" sqref="B7:B8 B5"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1981,10 +1984,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="B7:B8 B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2025,6 +2028,12 @@
       <c r="B5" s="5" t="s">
         <v>26</v>
       </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2048,8 +2057,8 @@
   </sheetPr>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7:B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2069,7 +2078,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>26</v>
@@ -2077,7 +2086,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>26</v>
@@ -2085,7 +2094,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>26</v>
@@ -2093,7 +2102,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>26</v>
@@ -2101,7 +2110,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>26</v>
@@ -2109,7 +2118,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>26</v>
@@ -2138,7 +2147,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B7:B8"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2158,7 +2167,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>26</v>
@@ -2166,7 +2175,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>26</v>
@@ -2174,7 +2183,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>26</v>
@@ -2182,7 +2191,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>26</v>
@@ -2190,7 +2199,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B7" s="5"/>
     </row>
@@ -2217,7 +2226,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I41" activeCellId="1" sqref="B7:B8 I41"/>
+      <selection pane="topLeft" activeCell="I41" activeCellId="0" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2237,7 +2246,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>26</v>
@@ -2245,7 +2254,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>27</v>
@@ -2253,7 +2262,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>27</v>
@@ -2261,7 +2270,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Added more function pointer test cases (#449)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -13,10 +13,11 @@
     <sheet name="Built-in functions" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Error handling" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Function calling" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Memory allocation" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Thread handling" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="Package manager" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="Iterator" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Function pointer" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Memory allocation" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Thread handling" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Package manager" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Iterator" sheetId="10" state="visible" r:id="rId11"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="95">
   <si>
     <t xml:space="preserve">Context</t>
   </si>
@@ -241,6 +242,21 @@
   </si>
   <si>
     <t xml:space="preserve">Return const pointer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Free function thunk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Floatng point args</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Struct args</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Array args</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slice args</t>
   </si>
   <si>
     <t xml:space="preserve">Create internal slice</t>
@@ -1581,6 +1597,80 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I41" activeCellId="0" sqref="I41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="9"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="9"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -1984,15 +2074,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.06"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2033,8 +2123,42 @@
       <c r="A6" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="5"/>
-    </row>
+      <c r="B6" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:A2"/>
@@ -2055,13 +2179,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.1"/>
   </cols>
@@ -2078,7 +2202,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>26</v>
@@ -2086,7 +2210,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>26</v>
@@ -2094,7 +2218,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>26</v>
@@ -2102,27 +2226,9 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="B6" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2144,13 +2250,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.1"/>
   </cols>
@@ -2167,7 +2273,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>26</v>
@@ -2175,7 +2281,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>26</v>
@@ -2183,7 +2289,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>26</v>
@@ -2191,7 +2297,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>26</v>
@@ -2199,9 +2305,19 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="5"/>
+      <c r="B8" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2223,10 +2339,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I41" activeCellId="0" sqref="I41"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2257,7 +2373,7 @@
         <v>87</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2265,7 +2381,7 @@
         <v>88</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2276,7 +2392,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B7" s="5"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:A2"/>

</xml_diff>

<commit_message>
Restored omit-functions options (#481)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integration/test-matrix.xlsx
+++ b/zigar-compiler/test/integration/test-matrix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Type handling" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,6 +18,7 @@
     <sheet name="Thread handling" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="Package manager" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="Iterator" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Options" sheetId="11" state="visible" r:id="rId12"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="97">
   <si>
     <t xml:space="preserve">Context</t>
   </si>
@@ -314,6 +315,12 @@
   </si>
   <si>
     <t xml:space="preserve">std.fs.path.ComponentIterator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Omitting functions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Omitting variables</t>
   </si>
 </sst>
 </file>
@@ -1671,6 +1678,64 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="9"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="9"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -1868,7 +1933,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2076,7 +2141,7 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -2252,8 +2317,8 @@
   </sheetPr>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>